<commit_message>
Minor mistake corrected, results updated
</commit_message>
<xml_diff>
--- a/Output/AppendixTab5.xlsx
+++ b/Output/AppendixTab5.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I59"/>
+  <dimension ref="A1:I115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -414,19 +414,19 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ES21.03.2020</t>
+          <t>DE_21.03.2020</t>
         </is>
       </c>
       <c r="C2" s="2">
         <v>43911</v>
       </c>
       <c r="D2">
-        <v>0.06019179616407672</v>
+        <v>0.01779010640067703</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -441,1882 +441,3730 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ES22.03.2020</t>
+          <t>DE_22.03.2020</t>
         </is>
       </c>
       <c r="C3" s="2">
         <v>43912</v>
       </c>
       <c r="D3">
-        <v>0.06594316557416188</v>
+        <v>0.01898596689403485</v>
       </c>
       <c r="E3">
-        <v>0.00575136941008516</v>
+        <v>0.001195860493357816</v>
       </c>
       <c r="F3">
-        <v>-3.858079447994556e-006</v>
+        <v>0.0006809749060308032</v>
       </c>
       <c r="G3">
-        <v>0.005755227489533162</v>
+        <v>0.0005148855873270133</v>
       </c>
       <c r="H3">
-        <v>0.0006699118118290245</v>
+        <v>0.5694434340904738</v>
       </c>
       <c r="I3">
-        <v>0.9993300881881709</v>
+        <v>0.4305565659095263</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ES23.03.2020</t>
+          <t>DE_23.03.2020</t>
         </is>
       </c>
       <c r="C4" s="2">
         <v>43913</v>
       </c>
       <c r="D4">
-        <v>0.06795822841284606</v>
+        <v>0.02074126468516609</v>
       </c>
       <c r="E4">
-        <v>0.007766432248769321</v>
+        <v>0.002951158284489056</v>
       </c>
       <c r="F4">
-        <v>-0.001310582187524533</v>
+        <v>0.00161521463948331</v>
       </c>
       <c r="G4">
-        <v>0.009077014436293862</v>
+        <v>0.001335943645005747</v>
       </c>
       <c r="H4">
-        <v>0.1261679900545439</v>
+        <v>0.5473154889633299</v>
       </c>
       <c r="I4">
-        <v>0.8738320099454561</v>
+        <v>0.4526845110366701</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ES24.03.2020</t>
+          <t>DE_24.03.2020</t>
         </is>
       </c>
       <c r="C5" s="2">
         <v>43914</v>
       </c>
       <c r="D5">
-        <v>0.07212770426381013</v>
+        <v>0.02239755002465547</v>
       </c>
       <c r="E5">
-        <v>0.0119359080997334</v>
+        <v>0.004607443623978445</v>
       </c>
       <c r="F5">
-        <v>-0.0005477051993754985</v>
+        <v>0.003006176338122966</v>
       </c>
       <c r="G5">
-        <v>0.0124836132991089</v>
+        <v>0.001601267285855478</v>
       </c>
       <c r="H5">
-        <v>0.04202991427453785</v>
+        <v>0.6524607968023681</v>
       </c>
       <c r="I5">
-        <v>0.9579700857254622</v>
+        <v>0.3475392031976319</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ES25.03.2020</t>
+          <t>DE_25.03.2020</t>
         </is>
       </c>
       <c r="C6" s="2">
         <v>43915</v>
       </c>
       <c r="D6">
-        <v>0.0727735459528725</v>
+        <v>0.02435775667118951</v>
       </c>
       <c r="E6">
-        <v>0.01258174978879578</v>
+        <v>0.006567650270512478</v>
       </c>
       <c r="F6">
-        <v>0.001038486619041438</v>
+        <v>0.004202196221316183</v>
       </c>
       <c r="G6">
-        <v>0.01154326316975435</v>
+        <v>0.002365454049196297</v>
       </c>
       <c r="H6">
-        <v>0.08253912504016124</v>
+        <v>0.6398325197343801</v>
       </c>
       <c r="I6">
-        <v>0.9174608749598388</v>
+        <v>0.3601674802656199</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ES26.03.2020</t>
+          <t>DE_26.03.2020</t>
         </is>
       </c>
       <c r="C7" s="2">
         <v>43916</v>
       </c>
       <c r="D7">
-        <v>0.07583778104906251</v>
+        <v>0.02669052277999517</v>
       </c>
       <c r="E7">
-        <v>0.01564598488498579</v>
+        <v>0.008900416379318141</v>
       </c>
       <c r="F7">
-        <v>0.001337085291855043</v>
+        <v>0.005747527036662928</v>
       </c>
       <c r="G7">
-        <v>0.01430889959313074</v>
+        <v>0.003152889342655215</v>
       </c>
       <c r="H7">
-        <v>0.08545868487564101</v>
+        <v>0.6457593433514448</v>
       </c>
       <c r="I7">
-        <v>0.914541315124359</v>
+        <v>0.3542406566485552</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ES27.03.2020</t>
+          <t>DE_27.03.2020</t>
         </is>
       </c>
       <c r="C8" s="2">
         <v>43917</v>
       </c>
       <c r="D8">
-        <v>0.07875639636198047</v>
+        <v>0.02848621654798152</v>
       </c>
       <c r="E8">
-        <v>0.01856460019790373</v>
+        <v>0.01069611014730449</v>
       </c>
       <c r="F8">
-        <v>0.001365190063536668</v>
+        <v>0.007467057853827177</v>
       </c>
       <c r="G8">
-        <v>0.01719941013436706</v>
+        <v>0.003229052293477318</v>
       </c>
       <c r="H8">
-        <v>0.07353727249622222</v>
+        <v>0.6981096633254974</v>
       </c>
       <c r="I8">
-        <v>0.9264627275037778</v>
+        <v>0.3018903366745027</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ES28.03.2020</t>
+          <t>DE_28.03.2020</t>
         </is>
       </c>
       <c r="C9" s="2">
         <v>43918</v>
       </c>
       <c r="D9">
-        <v>0.08284568848345941</v>
+        <v>0.03036122962980001</v>
       </c>
       <c r="E9">
-        <v>0.02265389231938269</v>
+        <v>0.01257112322912298</v>
       </c>
       <c r="F9">
-        <v>-0.0004790254947458016</v>
+        <v>0.009019506788199232</v>
       </c>
       <c r="G9">
-        <v>0.0231329178141285</v>
+        <v>0.003551616440923747</v>
       </c>
       <c r="H9">
-        <v>0.0202874235500034</v>
+        <v>0.7174781937785901</v>
       </c>
       <c r="I9">
-        <v>0.9797125764499967</v>
+        <v>0.2825218062214099</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ES29.03.2020</t>
+          <t>DE_29.03.2020</t>
         </is>
       </c>
       <c r="C10" s="2">
         <v>43919</v>
       </c>
       <c r="D10">
-        <v>0.08615539193073764</v>
+        <v>0.03142839719865093</v>
       </c>
       <c r="E10">
-        <v>0.02596359576666091</v>
+        <v>0.0136382907979739</v>
       </c>
       <c r="F10">
-        <v>-0.0008341553100068579</v>
+        <v>0.009839950521922125</v>
       </c>
       <c r="G10">
-        <v>0.02679775107666779</v>
+        <v>0.00379834027605177</v>
       </c>
       <c r="H10">
-        <v>0.03018812015117153</v>
+        <v>0.7214944062773576</v>
       </c>
       <c r="I10">
-        <v>0.9698118798488286</v>
+        <v>0.2785055937226424</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ES30.03.2020</t>
+          <t>DE_30.03.2020</t>
         </is>
       </c>
       <c r="C11" s="2">
         <v>43920</v>
       </c>
       <c r="D11">
-        <v>0.08673226219854474</v>
+        <v>0.03335972420316955</v>
       </c>
       <c r="E11">
-        <v>0.02654046603446802</v>
+        <v>0.01556961780249251</v>
       </c>
       <c r="F11">
-        <v>0.0003401292430913366</v>
+        <v>0.01124319127455804</v>
       </c>
       <c r="G11">
-        <v>0.02620033679137669</v>
+        <v>0.004326426527934474</v>
       </c>
       <c r="H11">
-        <v>0.01281549625577831</v>
+        <v>0.7221237808906355</v>
       </c>
       <c r="I11">
-        <v>0.9871845037442217</v>
+        <v>0.2778762191093647</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ES31.03.2020</t>
+          <t>DE_31.03.2020</t>
         </is>
       </c>
       <c r="C12" s="2">
         <v>43921</v>
       </c>
       <c r="D12">
-        <v>0.08863663288494469</v>
+        <v>0.03565074410643157</v>
       </c>
       <c r="E12">
-        <v>0.02844483672086796</v>
+        <v>0.01786063770575454</v>
       </c>
       <c r="F12">
-        <v>0.000524294472403285</v>
+        <v>0.01310006696188686</v>
       </c>
       <c r="G12">
-        <v>0.02792054224846468</v>
+        <v>0.004760570743867675</v>
       </c>
       <c r="H12">
-        <v>0.01843197335067307</v>
+        <v>0.7334602032527731</v>
       </c>
       <c r="I12">
-        <v>0.981568026649327</v>
+        <v>0.2665397967472271</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>ES01.04.2020</t>
+          <t>DE_01.04.2020</t>
         </is>
       </c>
       <c r="C13" s="2">
         <v>43922</v>
       </c>
       <c r="D13">
-        <v>0.09074011750949537</v>
+        <v>0.03749284985948419</v>
       </c>
       <c r="E13">
-        <v>0.03054832134541865</v>
+        <v>0.01970274345880716</v>
       </c>
       <c r="F13">
-        <v>0.003201087869198089</v>
+        <v>0.01493734594320361</v>
       </c>
       <c r="G13">
-        <v>0.02734723347622057</v>
+        <v>0.004765397515603554</v>
       </c>
       <c r="H13">
-        <v>0.1047876848289786</v>
+        <v>0.7581353314797685</v>
       </c>
       <c r="I13">
-        <v>0.8952123151710214</v>
+        <v>0.2418646685202315</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ES02.04.2020</t>
+          <t>DE_02.04.2020</t>
         </is>
       </c>
       <c r="C14" s="2">
         <v>43923</v>
       </c>
       <c r="D14">
-        <v>0.09289687121156129</v>
+        <v>0.03943299265373694</v>
       </c>
       <c r="E14">
-        <v>0.03270507504748457</v>
+        <v>0.02164288625305991</v>
       </c>
       <c r="F14">
-        <v>0.003336131809757762</v>
+        <v>0.016865312869742</v>
       </c>
       <c r="G14">
-        <v>0.0293689432377268</v>
+        <v>0.004777573383317908</v>
       </c>
       <c r="H14">
-        <v>0.1020065480636881</v>
+        <v>0.7792543320028563</v>
       </c>
       <c r="I14">
-        <v>0.8979934519363119</v>
+        <v>0.2207456679971437</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ES03.04.2020</t>
+          <t>DE_03.04.2020</t>
         </is>
       </c>
       <c r="C15" s="2">
         <v>43924</v>
       </c>
       <c r="D15">
-        <v>0.09415164828116983</v>
+        <v>0.04096964388643266</v>
       </c>
       <c r="E15">
-        <v>0.03395985211709311</v>
+        <v>0.02317953748575562</v>
       </c>
       <c r="F15">
-        <v>0.003356115487436793</v>
+        <v>0.0186705309769666</v>
       </c>
       <c r="G15">
-        <v>0.03060373662965633</v>
+        <v>0.004509006508789018</v>
       </c>
       <c r="H15">
-        <v>0.09882597473819826</v>
+        <v>0.8054746988994103</v>
       </c>
       <c r="I15">
-        <v>0.9011740252618018</v>
+        <v>0.1945253011005898</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ES04.04.2020</t>
+          <t>DE_04.04.2020</t>
         </is>
       </c>
       <c r="C16" s="2">
         <v>43925</v>
       </c>
       <c r="D16">
-        <v>0.09496860636743934</v>
+        <v>0.041660256607489</v>
       </c>
       <c r="E16">
-        <v>0.03477681020336262</v>
+        <v>0.02387015020681197</v>
       </c>
       <c r="F16">
-        <v>0.002525581978059256</v>
+        <v>0.01960218539733611</v>
       </c>
       <c r="G16">
-        <v>0.03225122822530336</v>
+        <v>0.00426796480947586</v>
       </c>
       <c r="H16">
-        <v>0.07262258853789454</v>
+        <v>0.8212007560699017</v>
       </c>
       <c r="I16">
-        <v>0.9273774114621054</v>
+        <v>0.1787992439300983</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ES05.04.2020</t>
+          <t>DE_05.04.2020</t>
         </is>
       </c>
       <c r="C17" s="2">
         <v>43926</v>
       </c>
       <c r="D17">
-        <v>0.09668085837494697</v>
+        <v>0.04241535667777022</v>
       </c>
       <c r="E17">
-        <v>0.03648906221087025</v>
+        <v>0.02462525027709319</v>
       </c>
       <c r="F17">
-        <v>0.002580556368032315</v>
+        <v>0.0203063905230269</v>
       </c>
       <c r="G17">
-        <v>0.03390850584283793</v>
+        <v>0.004318859754066284</v>
       </c>
       <c r="H17">
-        <v>0.0707213672173673</v>
+        <v>0.8246166148376669</v>
       </c>
       <c r="I17">
-        <v>0.9292786327826327</v>
+        <v>0.1753833851623331</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>ES06.04.2020</t>
+          <t>DE_06.04.2020</t>
         </is>
       </c>
       <c r="C18" s="2">
         <v>43927</v>
       </c>
       <c r="D18">
-        <v>0.09820012810476123</v>
+        <v>0.04368992875803762</v>
       </c>
       <c r="E18">
-        <v>0.0380083319406845</v>
+        <v>0.02589982235736059</v>
       </c>
       <c r="F18">
-        <v>0.002714690879364489</v>
+        <v>0.02135282900240082</v>
       </c>
       <c r="G18">
-        <v>0.03529364106132002</v>
+        <v>0.004546993354959767</v>
       </c>
       <c r="H18">
-        <v>0.07142357322076154</v>
+        <v>0.8244392068709485</v>
       </c>
       <c r="I18">
-        <v>0.9285764267792385</v>
+        <v>0.1755607931290516</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>ES07.04.2020</t>
+          <t>DE_07.04.2020</t>
         </is>
       </c>
       <c r="C19" s="2">
         <v>43928</v>
       </c>
       <c r="D19">
-        <v>0.09922278326894589</v>
+        <v>0.04467006940109426</v>
       </c>
       <c r="E19">
-        <v>0.03903098710486917</v>
+        <v>0.02687996300041723</v>
       </c>
       <c r="F19">
-        <v>0.004169707218563959</v>
+        <v>0.0223334860039112</v>
       </c>
       <c r="G19">
-        <v>0.03486127988630521</v>
+        <v>0.004546476996506025</v>
       </c>
       <c r="H19">
-        <v>0.1068306883287556</v>
+        <v>0.8308599979681722</v>
       </c>
       <c r="I19">
-        <v>0.8931693116712444</v>
+        <v>0.1691400020318278</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ES08.04.2020</t>
+          <t>DE_08.04.2020</t>
         </is>
       </c>
       <c r="C20" s="2">
         <v>43929</v>
       </c>
       <c r="D20">
-        <v>0.09995611557936292</v>
+        <v>0.04552988322685091</v>
       </c>
       <c r="E20">
-        <v>0.03976431941528619</v>
+        <v>0.02773977682617388</v>
       </c>
       <c r="F20">
-        <v>0.006298452280151913</v>
+        <v>0.02336861516234134</v>
       </c>
       <c r="G20">
-        <v>0.03346586713513429</v>
+        <v>0.004371161663832533</v>
       </c>
       <c r="H20">
-        <v>0.1583945701263697</v>
+        <v>0.8424226088326665</v>
       </c>
       <c r="I20">
-        <v>0.8416054298736304</v>
+        <v>0.1575773911673335</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>ES09.04.2020</t>
+          <t>DE_09.04.2020</t>
         </is>
       </c>
       <c r="C21" s="2">
         <v>43930</v>
       </c>
       <c r="D21">
-        <v>0.1008961812945718</v>
+        <v>0.04636423162807878</v>
       </c>
       <c r="E21">
-        <v>0.04070438513049512</v>
+        <v>0.02857412522740175</v>
       </c>
       <c r="F21">
-        <v>0.007215201159022493</v>
+        <v>0.02430038636348878</v>
       </c>
       <c r="G21">
-        <v>0.03348918397147263</v>
+        <v>0.004273738863912972</v>
       </c>
       <c r="H21">
-        <v>0.1772585714264228</v>
+        <v>0.8504332563148922</v>
       </c>
       <c r="I21">
-        <v>0.8227414285735771</v>
+        <v>0.1495667436851079</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>ES10.04.2020</t>
+          <t>DE_10.04.2020</t>
         </is>
       </c>
       <c r="C22" s="2">
         <v>43931</v>
       </c>
       <c r="D22">
-        <v>0.1010379228938024</v>
+        <v>0.04678698250458675</v>
       </c>
       <c r="E22">
-        <v>0.0408461267297257</v>
+        <v>0.02899687610390972</v>
       </c>
       <c r="F22">
-        <v>0.00750685463771595</v>
+        <v>0.02499841021740376</v>
       </c>
       <c r="G22">
-        <v>0.03333927209200975</v>
+        <v>0.003998465886505968</v>
       </c>
       <c r="H22">
-        <v>0.1837837572063558</v>
+        <v>0.8621070120733853</v>
       </c>
       <c r="I22">
-        <v>0.8162162427936441</v>
+        <v>0.1378929879266148</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ES11.04.2020</t>
+          <t>DE_11.04.2020</t>
         </is>
       </c>
       <c r="C23" s="2">
         <v>43932</v>
       </c>
       <c r="D23">
-        <v>0.1022292629156904</v>
+        <v>0.04727867063587024</v>
       </c>
       <c r="E23">
-        <v>0.04203746675161365</v>
+        <v>0.02948856423519321</v>
       </c>
       <c r="F23">
-        <v>0.007887129787960185</v>
+        <v>0.02567311617068808</v>
       </c>
       <c r="G23">
-        <v>0.03415033696365347</v>
+        <v>0.003815448064505129</v>
       </c>
       <c r="H23">
-        <v>0.1876214338642903</v>
+        <v>0.8706126200626759</v>
       </c>
       <c r="I23">
-        <v>0.8123785661357097</v>
+        <v>0.129387379937324</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ES13.04.2020</t>
+          <t>DE_12.04.2020</t>
         </is>
       </c>
       <c r="C24" s="2">
-        <v>43934</v>
+        <v>43933</v>
       </c>
       <c r="D24">
-        <v>0.104648568197875</v>
+        <v>0.04791322801226126</v>
       </c>
       <c r="E24">
-        <v>0.04445677203379821</v>
+        <v>0.03012312161158423</v>
       </c>
       <c r="F24">
-        <v>0.008137884379947558</v>
+        <v>0.02637482124111931</v>
       </c>
       <c r="G24">
-        <v>0.03631888765385066</v>
+        <v>0.003748300370464918</v>
       </c>
       <c r="H24">
-        <v>0.1830516253802849</v>
+        <v>0.8755673326690199</v>
       </c>
       <c r="I24">
-        <v>0.816948374619715</v>
+        <v>0.1244326673309801</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ES14.04.2020</t>
+          <t>DE_13.04.2020</t>
         </is>
       </c>
       <c r="C25" s="2">
-        <v>43935</v>
+        <v>43934</v>
       </c>
       <c r="D25">
-        <v>0.1045914303133819</v>
+        <v>0.04856857422525404</v>
       </c>
       <c r="E25">
-        <v>0.04439963414930518</v>
+        <v>0.03077846782457701</v>
       </c>
       <c r="F25">
-        <v>0.008309766262526967</v>
+        <v>0.02697230252412678</v>
       </c>
       <c r="G25">
-        <v>0.03608986788677821</v>
+        <v>0.003806165300450235</v>
       </c>
       <c r="H25">
-        <v>0.1871584399678439</v>
+        <v>0.8763367519740225</v>
       </c>
       <c r="I25">
-        <v>0.812841560032156</v>
+        <v>0.1236632480259775</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ES15.04.2020</t>
+          <t>DE_14.04.2020</t>
         </is>
       </c>
       <c r="C26" s="2">
-        <v>43936</v>
+        <v>43935</v>
       </c>
       <c r="D26">
-        <v>0.1046412786626991</v>
+        <v>0.04931756211251086</v>
       </c>
       <c r="E26">
-        <v>0.04444948249862239</v>
+        <v>0.03152745571183382</v>
       </c>
       <c r="F26">
-        <v>0.0120367114986402</v>
+        <v>0.02763426643980753</v>
       </c>
       <c r="G26">
-        <v>0.03241277099998218</v>
+        <v>0.003893189272026297</v>
       </c>
       <c r="H26">
-        <v>0.2707953123866685</v>
+        <v>0.8765143211171022</v>
       </c>
       <c r="I26">
-        <v>0.7292046876133315</v>
+        <v>0.1234856788828979</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ES16.04.2020</t>
+          <t>DE_15.04.2020</t>
         </is>
       </c>
       <c r="C27" s="2">
-        <v>43937</v>
+        <v>43936</v>
       </c>
       <c r="D27">
-        <v>0.1035688668094164</v>
+        <v>0.04977120104593807</v>
       </c>
       <c r="E27">
-        <v>0.04337707064533965</v>
+        <v>0.03198109464526104</v>
       </c>
       <c r="F27">
-        <v>0.01261866094284454</v>
+        <v>0.02827757941939385</v>
       </c>
       <c r="G27">
-        <v>0.03075840970249512</v>
+        <v>0.003703515225867196</v>
       </c>
       <c r="H27">
-        <v>0.290906249663963</v>
+        <v>0.8841967335093709</v>
       </c>
       <c r="I27">
-        <v>0.7090937503360369</v>
+        <v>0.1158032664906291</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ES17.04.2020</t>
+          <t>DE_16.04.2020</t>
         </is>
       </c>
       <c r="C28" s="2">
-        <v>43938</v>
+        <v>43937</v>
       </c>
       <c r="D28">
-        <v>0.1045402790752016</v>
+        <v>0.04988586236399292</v>
       </c>
       <c r="E28">
-        <v>0.04434848291112482</v>
+        <v>0.03209575596331589</v>
       </c>
       <c r="F28">
-        <v>0.01285210210924739</v>
+        <v>0.02849745372902557</v>
       </c>
       <c r="G28">
-        <v>0.03149638080187744</v>
+        <v>0.003598302234290324</v>
       </c>
       <c r="H28">
-        <v>0.2897980103401336</v>
+        <v>0.887888534596193</v>
       </c>
       <c r="I28">
-        <v>0.7102019896598665</v>
+        <v>0.1121114654038071</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ES18.04.2020</t>
+          <t>DE_17.04.2020</t>
         </is>
       </c>
       <c r="C29" s="2">
-        <v>43939</v>
+        <v>43938</v>
       </c>
       <c r="D29">
-        <v>0.1043813538562038</v>
+        <v>0.05003508622706105</v>
       </c>
       <c r="E29">
-        <v>0.04418955769212709</v>
+        <v>0.03224497982638402</v>
       </c>
       <c r="F29">
-        <v>0.01271188391315186</v>
+        <v>0.02878269963280154</v>
       </c>
       <c r="G29">
-        <v>0.03147767377897523</v>
+        <v>0.003462280193582476</v>
       </c>
       <c r="H29">
-        <v>0.2876671452952026</v>
+        <v>0.8926257602819304</v>
       </c>
       <c r="I29">
-        <v>0.7123328547047974</v>
+        <v>0.1073742397180696</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ES19.04.2020</t>
+          <t>DE_18.04.2020</t>
         </is>
       </c>
       <c r="C30" s="2">
-        <v>43940</v>
+        <v>43939</v>
       </c>
       <c r="D30">
-        <v>0.1041506418260826</v>
+        <v>0.05013723121189477</v>
       </c>
       <c r="E30">
-        <v>0.0439588456620059</v>
+        <v>0.03234712481121774</v>
       </c>
       <c r="F30">
-        <v>0.0130692689693004</v>
+        <v>0.02897740091784215</v>
       </c>
       <c r="G30">
-        <v>0.0308895766927055</v>
+        <v>0.00336972389337559</v>
       </c>
       <c r="H30">
-        <v>0.2973069190621698</v>
+        <v>0.8958261696196568</v>
       </c>
       <c r="I30">
-        <v>0.7026930809378303</v>
+        <v>0.1041738303803432</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ES20.04.2020</t>
+          <t>DE_19.04.2020</t>
         </is>
       </c>
       <c r="C31" s="2">
-        <v>43941</v>
+        <v>43940</v>
       </c>
       <c r="D31">
-        <v>0.1042330711438059</v>
+        <v>0.05047520889823474</v>
       </c>
       <c r="E31">
-        <v>0.04404127497972917</v>
+        <v>0.03268510249755771</v>
       </c>
       <c r="F31">
-        <v>0.01313913216593426</v>
+        <v>0.02930621718352507</v>
       </c>
       <c r="G31">
-        <v>0.03090214281379492</v>
+        <v>0.003378885314032648</v>
       </c>
       <c r="H31">
-        <v>0.2983367800314998</v>
+        <v>0.8966230773091465</v>
       </c>
       <c r="I31">
-        <v>0.7016632199685002</v>
+        <v>0.1033769226908536</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>ES21.04.2020</t>
+          <t>DE_20.04.2020</t>
         </is>
       </c>
       <c r="C32" s="2">
-        <v>43942</v>
+        <v>43941</v>
       </c>
       <c r="D32">
-        <v>0.104213804094172</v>
+        <v>0.05085246284894376</v>
       </c>
       <c r="E32">
-        <v>0.04402200793009529</v>
+        <v>0.03306235644826673</v>
       </c>
       <c r="F32">
-        <v>0.01381032490775763</v>
+        <v>0.02969152373185961</v>
       </c>
       <c r="G32">
-        <v>0.03021168302233766</v>
+        <v>0.003370832716407121</v>
       </c>
       <c r="H32">
-        <v>0.3137141070368195</v>
+        <v>0.898046204852896</v>
       </c>
       <c r="I32">
-        <v>0.6862858929631805</v>
+        <v>0.1019537951471041</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ES22.04.2020</t>
+          <t>DE_21.04.2020</t>
         </is>
       </c>
       <c r="C33" s="2">
-        <v>43943</v>
+        <v>43942</v>
       </c>
       <c r="D33">
-        <v>0.1040122239747634</v>
+        <v>0.05101027142394358</v>
       </c>
       <c r="E33">
-        <v>0.04382042781068669</v>
+        <v>0.03322016502326655</v>
       </c>
       <c r="F33">
-        <v>0.01397790755186786</v>
+        <v>0.02995726979908094</v>
       </c>
       <c r="G33">
-        <v>0.02984252025881883</v>
+        <v>0.003262895224185612</v>
       </c>
       <c r="H33">
-        <v>0.3189815401222304</v>
+        <v>0.901779680447091</v>
       </c>
       <c r="I33">
-        <v>0.6810184598777697</v>
+        <v>0.09822031955290904</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ES23.04.2020</t>
+          <t>DE_22.04.2020</t>
         </is>
       </c>
       <c r="C34" s="2">
-        <v>43944</v>
+        <v>43943</v>
       </c>
       <c r="D34">
-        <v>0.1109611310902015</v>
+        <v>0.05100841132080721</v>
       </c>
       <c r="E34">
-        <v>0.05076933492612475</v>
+        <v>0.03321830492013017</v>
       </c>
       <c r="F34">
-        <v>0.01440348005250176</v>
+        <v>0.03016939998894428</v>
       </c>
       <c r="G34">
-        <v>0.036365854873623</v>
+        <v>0.003048904931185902</v>
       </c>
       <c r="H34">
-        <v>0.2837043280842754</v>
+        <v>0.9082161194402706</v>
       </c>
       <c r="I34">
-        <v>0.7162956719157246</v>
+        <v>0.09178388055972946</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>ES24.04.2020</t>
+          <t>DE_23.04.2020</t>
         </is>
       </c>
       <c r="C35" s="2">
-        <v>43945</v>
+        <v>43944</v>
       </c>
       <c r="D35">
-        <v>0.1112260508486924</v>
+        <v>0.0510643357840399</v>
       </c>
       <c r="E35">
-        <v>0.05103425468461564</v>
+        <v>0.03327422938336287</v>
       </c>
       <c r="F35">
-        <v>0.01723963522217091</v>
+        <v>0.03045014815195636</v>
       </c>
       <c r="G35">
-        <v>0.03379461946244473</v>
+        <v>0.002824081231406509</v>
       </c>
       <c r="H35">
-        <v>0.3378051727944178</v>
+        <v>0.9151270733014015</v>
       </c>
       <c r="I35">
-        <v>0.6621948272055823</v>
+        <v>0.0848729266985985</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>ES25.04.2020</t>
+          <t>DE_24.04.2020</t>
         </is>
       </c>
       <c r="C36" s="2">
-        <v>43946</v>
+        <v>43945</v>
       </c>
       <c r="D36">
-        <v>0.1116874460288036</v>
+        <v>0.05098606836818124</v>
       </c>
       <c r="E36">
-        <v>0.05149564986472686</v>
+        <v>0.03319596196750421</v>
       </c>
       <c r="F36">
-        <v>0.01723914422351622</v>
+        <v>0.03050673958764946</v>
       </c>
       <c r="G36">
-        <v>0.03425650564121064</v>
+        <v>0.002689222379854744</v>
       </c>
       <c r="H36">
-        <v>0.3347689420135773</v>
+        <v>0.918989472801323</v>
       </c>
       <c r="I36">
-        <v>0.6652310579864228</v>
+        <v>0.08101052719867692</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>ES26.04.2020</t>
+          <t>DE_25.04.2020</t>
         </is>
       </c>
       <c r="C37" s="2">
-        <v>43947</v>
+        <v>43946</v>
       </c>
       <c r="D37">
-        <v>0.1122917373825043</v>
+        <v>0.0510567211561848</v>
       </c>
       <c r="E37">
-        <v>0.05209994121842756</v>
+        <v>0.03326661475550777</v>
       </c>
       <c r="F37">
-        <v>0.01790265674952325</v>
+        <v>0.0306526182185627</v>
       </c>
       <c r="G37">
-        <v>0.03419728446890432</v>
+        <v>0.002613996536945072</v>
       </c>
       <c r="H37">
-        <v>0.3436214385437952</v>
+        <v>0.9214228271750348</v>
       </c>
       <c r="I37">
-        <v>0.6563785614562049</v>
+        <v>0.07857717282496521</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ES27.04.2020</t>
+          <t>DE_26.04.2020</t>
         </is>
       </c>
       <c r="C38" s="2">
-        <v>43948</v>
+        <v>43947</v>
       </c>
       <c r="D38">
-        <v>0.1130225944606731</v>
+        <v>0.0510060716659201</v>
       </c>
       <c r="E38">
-        <v>0.05283079829659635</v>
+        <v>0.03321596526524308</v>
       </c>
       <c r="F38">
-        <v>0.01798604655531074</v>
+        <v>0.03070499970697992</v>
       </c>
       <c r="G38">
-        <v>0.03484475174128561</v>
+        <v>0.002510965558263158</v>
       </c>
       <c r="H38">
-        <v>0.3404462384674868</v>
+        <v>0.9244048595844779</v>
       </c>
       <c r="I38">
-        <v>0.6595537615325132</v>
+        <v>0.07559514041552218</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ES28.04.2020</t>
+          <t>DE_27.04.2020</t>
         </is>
       </c>
       <c r="C39" s="2">
-        <v>43949</v>
+        <v>43948</v>
       </c>
       <c r="D39">
-        <v>0.1140124489766205</v>
+        <v>0.05111582964680158</v>
       </c>
       <c r="E39">
-        <v>0.05382065281254374</v>
+        <v>0.03332572324612454</v>
       </c>
       <c r="F39">
-        <v>0.0179939354998141</v>
+        <v>0.03075039828718459</v>
       </c>
       <c r="G39">
-        <v>0.03582671731272966</v>
+        <v>0.002575324958939946</v>
       </c>
       <c r="H39">
-        <v>0.3343314240815066</v>
+        <v>0.9227226086011672</v>
       </c>
       <c r="I39">
-        <v>0.6656685759184934</v>
+        <v>0.07727739139883277</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>ES29.04.2020</t>
+          <t>DE_28.04.2020</t>
         </is>
       </c>
       <c r="C40" s="2">
-        <v>43950</v>
+        <v>43949</v>
       </c>
       <c r="D40">
-        <v>0.1149904584578638</v>
+        <v>0.05113533071968848</v>
       </c>
       <c r="E40">
-        <v>0.05479866229378706</v>
+        <v>0.03334522431901145</v>
       </c>
       <c r="F40">
-        <v>0.01809149595680683</v>
+        <v>0.03083404937868858</v>
       </c>
       <c r="G40">
-        <v>0.03670716633698023</v>
+        <v>0.002511174940322864</v>
       </c>
       <c r="H40">
-        <v>0.3301448465988923</v>
+        <v>0.9246916165175969</v>
       </c>
       <c r="I40">
-        <v>0.6698551534011077</v>
+        <v>0.075308383482403</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>ES30.04.2020</t>
+          <t>DE_29.04.2020</t>
         </is>
       </c>
       <c r="C41" s="2">
-        <v>43951</v>
+        <v>43950</v>
       </c>
       <c r="D41">
-        <v>0.1153441193963274</v>
+        <v>0.05104468895419274</v>
       </c>
       <c r="E41">
-        <v>0.05515232323225069</v>
+        <v>0.03325458255351571</v>
       </c>
       <c r="F41">
-        <v>0.01828232597111061</v>
+        <v>0.03088924498372474</v>
       </c>
       <c r="G41">
-        <v>0.03686999726114008</v>
+        <v>0.002365337569790972</v>
       </c>
       <c r="H41">
-        <v>0.331487866687362</v>
+        <v>0.9288718309428633</v>
       </c>
       <c r="I41">
-        <v>0.6685121333126382</v>
+        <v>0.07112816905713663</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>ES01.05.2020</t>
+          <t>DE_30.04.2020</t>
         </is>
       </c>
       <c r="C42" s="2">
-        <v>43952</v>
+        <v>43951</v>
       </c>
       <c r="D42">
-        <v>0.1158913871460292</v>
+        <v>0.05099892128322966</v>
       </c>
       <c r="E42">
-        <v>0.05569959098195242</v>
+        <v>0.03320881488255263</v>
       </c>
       <c r="F42">
-        <v>0.01822818417162254</v>
+        <v>0.03096774402868959</v>
       </c>
       <c r="G42">
-        <v>0.03747140681032989</v>
+        <v>0.002241070853863033</v>
       </c>
       <c r="H42">
-        <v>0.3272588514613827</v>
+        <v>0.9325157834813174</v>
       </c>
       <c r="I42">
-        <v>0.6727411485386173</v>
+        <v>0.06748421651868267</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>ES02.05.2020</t>
+          <t>DE_01.05.2020</t>
         </is>
       </c>
       <c r="C43" s="2">
-        <v>43953</v>
+        <v>43952</v>
       </c>
       <c r="D43">
-        <v>0.1161740226058326</v>
+        <v>0.05098818343231495</v>
       </c>
       <c r="E43">
-        <v>0.05598222644175591</v>
+        <v>0.03319807703163792</v>
       </c>
       <c r="F43">
-        <v>0.01826869142023503</v>
+        <v>0.03104146923539567</v>
       </c>
       <c r="G43">
-        <v>0.03771353502152089</v>
+        <v>0.002156607796242242</v>
       </c>
       <c r="H43">
-        <v>0.326330204806017</v>
+        <v>0.935038171211333</v>
       </c>
       <c r="I43">
-        <v>0.673669795193983</v>
+        <v>0.06496182878866705</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>ES03.05.2020</t>
+          <t>DE_02.05.2020</t>
         </is>
       </c>
       <c r="C44" s="2">
-        <v>43954</v>
+        <v>43953</v>
       </c>
       <c r="D44">
-        <v>0.1166367752085904</v>
+        <v>0.0509972119905753</v>
       </c>
       <c r="E44">
-        <v>0.05644497904451366</v>
+        <v>0.03320710558989827</v>
       </c>
       <c r="F44">
-        <v>0.01810401776534836</v>
+        <v>0.03105389296070132</v>
       </c>
       <c r="G44">
-        <v>0.03834096127916531</v>
+        <v>0.002153212629196947</v>
       </c>
       <c r="H44">
-        <v>0.3207374344327625</v>
+        <v>0.9351580756302964</v>
       </c>
       <c r="I44">
-        <v>0.6792625655672375</v>
+        <v>0.06484192436970368</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>ES04.05.2020</t>
+          <t>DE_03.05.2020</t>
         </is>
       </c>
       <c r="C45" s="2">
-        <v>43955</v>
+        <v>43954</v>
       </c>
       <c r="D45">
-        <v>0.1167793056188167</v>
+        <v>0.05095666171266507</v>
       </c>
       <c r="E45">
-        <v>0.05658750945473993</v>
+        <v>0.03316655531198805</v>
       </c>
       <c r="F45">
-        <v>0.01805635723718158</v>
+        <v>0.03099967622509332</v>
       </c>
       <c r="G45">
-        <v>0.03853115221755836</v>
+        <v>0.002166879086894724</v>
       </c>
       <c r="H45">
-        <v>0.3190873288322309</v>
+        <v>0.9346667428525053</v>
       </c>
       <c r="I45">
-        <v>0.6809126711677691</v>
+        <v>0.06533325714749479</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>ES05.05.2020</t>
+          <t>DE_04.05.2020</t>
         </is>
       </c>
       <c r="C46" s="2">
-        <v>43956</v>
+        <v>43955</v>
       </c>
       <c r="D46">
-        <v>0.117358901622603</v>
+        <v>0.05097485781430761</v>
       </c>
       <c r="E46">
-        <v>0.05716710545852625</v>
+        <v>0.03318475141363059</v>
       </c>
       <c r="F46">
-        <v>0.01816132311016618</v>
+        <v>0.03102616441175178</v>
       </c>
       <c r="G46">
-        <v>0.03900578234836007</v>
+        <v>0.002158587001878791</v>
       </c>
       <c r="H46">
-        <v>0.3176883448006985</v>
+        <v>0.9349524432178765</v>
       </c>
       <c r="I46">
-        <v>0.6823116551993016</v>
+        <v>0.06504755678212358</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>ES06.05.2020</t>
+          <t>DE_05.05.2020</t>
         </is>
       </c>
       <c r="C47" s="2">
-        <v>43957</v>
+        <v>43956</v>
       </c>
       <c r="D47">
-        <v>0.1177256328938153</v>
+        <v>0.05090020512678568</v>
       </c>
       <c r="E47">
-        <v>0.05753383672973853</v>
+        <v>0.03311009872610865</v>
       </c>
       <c r="F47">
-        <v>0.01784487861367573</v>
+        <v>0.03100841894845766</v>
       </c>
       <c r="G47">
-        <v>0.03968895811606281</v>
+        <v>0.002101679777650999</v>
       </c>
       <c r="H47">
-        <v>0.3101631948778402</v>
+        <v>0.9365245088806171</v>
       </c>
       <c r="I47">
-        <v>0.6898368051221598</v>
+        <v>0.06347549111938283</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>ES07.05.2020</t>
+          <t>DE_06.05.2020</t>
         </is>
       </c>
       <c r="C48" s="2">
-        <v>43958</v>
+        <v>43957</v>
       </c>
       <c r="D48">
-        <v>0.1180080132138606</v>
+        <v>0.05075895603968914</v>
       </c>
       <c r="E48">
-        <v>0.05781621704978383</v>
+        <v>0.0329688496390121</v>
       </c>
       <c r="F48">
-        <v>0.01798633102933133</v>
+        <v>0.03100872087370701</v>
       </c>
       <c r="G48">
-        <v>0.03982988602045251</v>
+        <v>0.001960128765305088</v>
       </c>
       <c r="H48">
-        <v>0.311094913280885</v>
+        <v>0.9405460370389853</v>
       </c>
       <c r="I48">
-        <v>0.6889050867191151</v>
+        <v>0.0594539629610147</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ES08.05.2020</t>
+          <t>DE_07.05.2020</t>
         </is>
       </c>
       <c r="C49" s="2">
-        <v>43959</v>
+        <v>43958</v>
       </c>
       <c r="D49">
-        <v>0.1184289681583019</v>
+        <v>0.05067112700700487</v>
       </c>
       <c r="E49">
-        <v>0.05823717199422516</v>
+        <v>0.03288102060632785</v>
       </c>
       <c r="F49">
-        <v>0.01801603161983535</v>
+        <v>0.0309871379838098</v>
       </c>
       <c r="G49">
-        <v>0.04022114037438981</v>
+        <v>0.001893882622518043</v>
       </c>
       <c r="H49">
-        <v>0.3093562239186654</v>
+        <v>0.942401951411643</v>
       </c>
       <c r="I49">
-        <v>0.6906437760813347</v>
+        <v>0.05759804858835713</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>ES09.05.2020</t>
+          <t>DE_08.05.2020</t>
         </is>
       </c>
       <c r="C50" s="2">
-        <v>43960</v>
+        <v>43959</v>
       </c>
       <c r="D50">
-        <v>0.1186371941708632</v>
+        <v>0.0506191621851118</v>
       </c>
       <c r="E50">
-        <v>0.0584453980067865</v>
+        <v>0.03282905578443478</v>
       </c>
       <c r="F50">
-        <v>0.01917400079928798</v>
+        <v>0.03098146040616766</v>
       </c>
       <c r="G50">
-        <v>0.03927139720749853</v>
+        <v>0.001847595378267109</v>
       </c>
       <c r="H50">
-        <v>0.3280669043790506</v>
+        <v>0.9437207274434282</v>
       </c>
       <c r="I50">
-        <v>0.6719330956209494</v>
+        <v>0.05627927255657193</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>ES10.05.2020</t>
+          <t>DE_09.05.2020</t>
         </is>
       </c>
       <c r="C51" s="2">
-        <v>43961</v>
+        <v>43960</v>
       </c>
       <c r="D51">
-        <v>0.1175891239733376</v>
+        <v>0.05055179340197225</v>
       </c>
       <c r="E51">
-        <v>0.05739732780926083</v>
+        <v>0.03276168700129521</v>
       </c>
       <c r="F51">
-        <v>0.01923405086130865</v>
+        <v>0.03094680847464078</v>
       </c>
       <c r="G51">
-        <v>0.03816327694795219</v>
+        <v>0.001814878526654428</v>
       </c>
       <c r="H51">
-        <v>0.3351035944604605</v>
+        <v>0.9446036302531466</v>
       </c>
       <c r="I51">
-        <v>0.6648964055395396</v>
+        <v>0.05539636974685334</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>ES11.05.2020</t>
+          <t>DE_10.05.2020</t>
         </is>
       </c>
       <c r="C52" s="2">
-        <v>43962</v>
+        <v>43961</v>
       </c>
       <c r="D52">
-        <v>0.1180550804718677</v>
+        <v>0.05053251663198616</v>
       </c>
       <c r="E52">
-        <v>0.05786328430779101</v>
+        <v>0.03274241023130914</v>
       </c>
       <c r="F52">
-        <v>0.01870533374320034</v>
+        <v>0.03092931474533325</v>
       </c>
       <c r="G52">
-        <v>0.03915795056459068</v>
+        <v>0.001813095485975889</v>
       </c>
       <c r="H52">
-        <v>0.323267750300889</v>
+        <v>0.9446254727991232</v>
       </c>
       <c r="I52">
-        <v>0.6767322496991109</v>
+        <v>0.05537452720087663</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>ES12.05.2020</t>
+          <t>DE_11.05.2020</t>
         </is>
       </c>
       <c r="C53" s="2">
-        <v>43963</v>
+        <v>43962</v>
       </c>
       <c r="D53">
-        <v>0.1185176148242016</v>
+        <v>0.05046582853726687</v>
       </c>
       <c r="E53">
-        <v>0.05832581866012485</v>
+        <v>0.03267572213658984</v>
       </c>
       <c r="F53">
-        <v>0.01872436282601783</v>
+        <v>0.0309025452329624</v>
       </c>
       <c r="G53">
-        <v>0.03960145583410702</v>
+        <v>0.001773176903627447</v>
       </c>
       <c r="H53">
-        <v>0.3210304331110738</v>
+        <v>0.9457341173298244</v>
       </c>
       <c r="I53">
-        <v>0.6789695668889263</v>
+        <v>0.05426588267017569</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>ES13.05.2020</t>
+          <t>DE_12.05.2020</t>
         </is>
       </c>
       <c r="C54" s="2">
-        <v>43964</v>
+        <v>43963</v>
       </c>
       <c r="D54">
-        <v>0.1190250583885416</v>
+        <v>0.05038718481866016</v>
       </c>
       <c r="E54">
-        <v>0.05883326222446488</v>
+        <v>0.03259707841798314</v>
       </c>
       <c r="F54">
-        <v>0.01859847548150096</v>
+        <v>0.03087518144653047</v>
       </c>
       <c r="G54">
-        <v>0.04023478674296391</v>
+        <v>0.001721896971452662</v>
       </c>
       <c r="H54">
-        <v>0.3161217783665085</v>
+        <v>0.947176340487535</v>
       </c>
       <c r="I54">
-        <v>0.6838782216334916</v>
+        <v>0.052823659512465</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>ES14.05.2020</t>
+          <t>DE_13.05.2020</t>
         </is>
       </c>
       <c r="C55" s="2">
-        <v>43965</v>
+        <v>43964</v>
       </c>
       <c r="D55">
-        <v>0.119292424161461</v>
+        <v>0.05026819064219537</v>
       </c>
       <c r="E55">
-        <v>0.0591006279973843</v>
+        <v>0.03247808424151834</v>
       </c>
       <c r="F55">
-        <v>0.01860153967493866</v>
+        <v>0.03085447683219634</v>
       </c>
       <c r="G55">
-        <v>0.04049908832244565</v>
+        <v>0.001623607409322004</v>
       </c>
       <c r="H55">
-        <v>0.3147435197433424</v>
+        <v>0.9500091385548392</v>
       </c>
       <c r="I55">
-        <v>0.6852564802566578</v>
+        <v>0.0499908614451608</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>ES15.05.2020</t>
+          <t>DE_14.05.2020</t>
         </is>
       </c>
       <c r="C56" s="2">
-        <v>43966</v>
+        <v>43965</v>
       </c>
       <c r="D56">
-        <v>0.1194769785607157</v>
+        <v>0.05015045712389027</v>
       </c>
       <c r="E56">
-        <v>0.05928518239663901</v>
+        <v>0.03236035072321324</v>
       </c>
       <c r="F56">
-        <v>0.01873318636473028</v>
+        <v>0.03084743147715913</v>
       </c>
       <c r="G56">
-        <v>0.04055199603190874</v>
+        <v>0.001512919246054105</v>
       </c>
       <c r="H56">
-        <v>0.3159842916464113</v>
+        <v>0.9532477487962195</v>
       </c>
       <c r="I56">
-        <v>0.6840157083535886</v>
+        <v>0.0467522512037805</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>ES16.05.2020</t>
+          <t>DE_15.05.2020</t>
         </is>
       </c>
       <c r="C57" s="2">
-        <v>43967</v>
+        <v>43966</v>
       </c>
       <c r="D57">
-        <v>0.1195159366829206</v>
+        <v>0.05011200293327375</v>
       </c>
       <c r="E57">
-        <v>0.05932414051884383</v>
+        <v>0.03232189653259672</v>
       </c>
       <c r="F57">
-        <v>0.01873584391753624</v>
+        <v>0.0308526509463183</v>
       </c>
       <c r="G57">
-        <v>0.0405882966013076</v>
+        <v>0.001469245586278421</v>
       </c>
       <c r="H57">
-        <v>0.3158215821362796</v>
+        <v>0.9545433361313844</v>
       </c>
       <c r="I57">
-        <v>0.6841784178637204</v>
+        <v>0.04545666386861558</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>ES17.05.2020</t>
+          <t>DE_16.05.2020</t>
         </is>
       </c>
       <c r="C58" s="2">
-        <v>43968</v>
+        <v>43967</v>
       </c>
       <c r="D58">
-        <v>0.1196390074691534</v>
+        <v>0.05008282284482044</v>
       </c>
       <c r="E58">
-        <v>0.05944721130507671</v>
+        <v>0.03229271644414342</v>
       </c>
       <c r="F58">
-        <v>0.01874477310959271</v>
+        <v>0.0308528295714661</v>
       </c>
       <c r="G58">
-        <v>0.04070243819548399</v>
+        <v>0.001439886872677319</v>
       </c>
       <c r="H58">
-        <v>0.3153179551753328</v>
+        <v>0.9554114044519021</v>
       </c>
       <c r="I58">
-        <v>0.6846820448246672</v>
+        <v>0.04458859554809785</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>ES21.05.2020</t>
+          <t>DE_17.05.2020</t>
         </is>
       </c>
       <c r="C59" s="2">
+        <v>43968</v>
+      </c>
+      <c r="D59">
+        <v>0.05003792912671751</v>
+      </c>
+      <c r="E59">
+        <v>0.03224782272604047</v>
+      </c>
+      <c r="F59">
+        <v>0.03079660969731902</v>
+      </c>
+      <c r="G59">
+        <v>0.00145121302872146</v>
+      </c>
+      <c r="H59">
+        <v>0.954998108211827</v>
+      </c>
+      <c r="I59">
+        <v>0.04500189178817301</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>DE_18.05.2020</t>
+        </is>
+      </c>
+      <c r="C60" s="2">
+        <v>43969</v>
+      </c>
+      <c r="D60">
+        <v>0.05000258712498771</v>
+      </c>
+      <c r="E60">
+        <v>0.03221248072431068</v>
+      </c>
+      <c r="F60">
+        <v>0.03075885635448205</v>
+      </c>
+      <c r="G60">
+        <v>0.001453624369828627</v>
+      </c>
+      <c r="H60">
+        <v>0.9548738769215133</v>
+      </c>
+      <c r="I60">
+        <v>0.0451261230784868</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>DE_19.05.2020</t>
+        </is>
+      </c>
+      <c r="C61" s="2">
+        <v>43970</v>
+      </c>
+      <c r="D61">
+        <v>0.04994903621826089</v>
+      </c>
+      <c r="E61">
+        <v>0.03215892981758386</v>
+      </c>
+      <c r="F61">
+        <v>0.03075924462181391</v>
+      </c>
+      <c r="G61">
+        <v>0.001399685195769947</v>
+      </c>
+      <c r="H61">
+        <v>0.9564760020401976</v>
+      </c>
+      <c r="I61">
+        <v>0.04352399795980235</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>DE_20.05.2020</t>
+        </is>
+      </c>
+      <c r="C62" s="2">
+        <v>43971</v>
+      </c>
+      <c r="D62">
+        <v>0.04984103240729521</v>
+      </c>
+      <c r="E62">
+        <v>0.03205092600661817</v>
+      </c>
+      <c r="F62">
+        <v>0.03068713414761496</v>
+      </c>
+      <c r="G62">
+        <v>0.001363791859003213</v>
+      </c>
+      <c r="H62">
+        <v>0.9574492213197957</v>
+      </c>
+      <c r="I62">
+        <v>0.04255077868020426</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>DE_21.05.2020</t>
+        </is>
+      </c>
+      <c r="C63" s="2">
         <v>43972</v>
       </c>
-      <c r="D59">
-        <v>0.121913536873179</v>
-      </c>
-      <c r="E59">
-        <v>0.06172174070910224</v>
-      </c>
-      <c r="F59">
-        <v>0.01964701438874281</v>
-      </c>
-      <c r="G59">
-        <v>0.04207472632035943</v>
-      </c>
-      <c r="H59">
-        <v>0.3183159477199485</v>
-      </c>
-      <c r="I59">
-        <v>0.6816840522800515</v>
+      <c r="D63">
+        <v>0.04975821506488833</v>
+      </c>
+      <c r="E63">
+        <v>0.03196810866421129</v>
+      </c>
+      <c r="F63">
+        <v>0.03065698686916141</v>
+      </c>
+      <c r="G63">
+        <v>0.00131112179504988</v>
+      </c>
+      <c r="H63">
+        <v>0.958986569746064</v>
+      </c>
+      <c r="I63">
+        <v>0.04101343025393609</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>DE_22.05.2020</t>
+        </is>
+      </c>
+      <c r="C64" s="2">
+        <v>43973</v>
+      </c>
+      <c r="D64">
+        <v>0.04967733001590504</v>
+      </c>
+      <c r="E64">
+        <v>0.03188722361522801</v>
+      </c>
+      <c r="F64">
+        <v>0.03062165146463812</v>
+      </c>
+      <c r="G64">
+        <v>0.001265572150589889</v>
+      </c>
+      <c r="H64">
+        <v>0.9603109958439435</v>
+      </c>
+      <c r="I64">
+        <v>0.03968900415605654</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>DE_23.05.2020</t>
+        </is>
+      </c>
+      <c r="C65" s="2">
+        <v>43974</v>
+      </c>
+      <c r="D65">
+        <v>0.04963938561537786</v>
+      </c>
+      <c r="E65">
+        <v>0.03184927921470084</v>
+      </c>
+      <c r="F65">
+        <v>0.03061666392874242</v>
+      </c>
+      <c r="G65">
+        <v>0.001232615285958417</v>
+      </c>
+      <c r="H65">
+        <v>0.9612984872389365</v>
+      </c>
+      <c r="I65">
+        <v>0.03870151276106343</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>DE_24.05.2020</t>
+        </is>
+      </c>
+      <c r="C66" s="2">
+        <v>43975</v>
+      </c>
+      <c r="D66">
+        <v>0.049604295659687</v>
+      </c>
+      <c r="E66">
+        <v>0.03181418925900997</v>
+      </c>
+      <c r="F66">
+        <v>0.03060802833988125</v>
+      </c>
+      <c r="G66">
+        <v>0.001206160919128716</v>
+      </c>
+      <c r="H66">
+        <v>0.962087328100397</v>
+      </c>
+      <c r="I66">
+        <v>0.03791267189960291</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>DE_25.05.2020</t>
+        </is>
+      </c>
+      <c r="C67" s="2">
+        <v>43976</v>
+      </c>
+      <c r="D67">
+        <v>0.04955814188192695</v>
+      </c>
+      <c r="E67">
+        <v>0.03176803548124992</v>
+      </c>
+      <c r="F67">
+        <v>0.03059261041440278</v>
+      </c>
+      <c r="G67">
+        <v>0.001175425066847136</v>
+      </c>
+      <c r="H67">
+        <v>0.9629997559168902</v>
+      </c>
+      <c r="I67">
+        <v>0.03700024408310969</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>DE_26.05.2020</t>
+        </is>
+      </c>
+      <c r="C68" s="2">
+        <v>43977</v>
+      </c>
+      <c r="D68">
+        <v>0.04947126845559266</v>
+      </c>
+      <c r="E68">
+        <v>0.03168116205491563</v>
+      </c>
+      <c r="F68">
+        <v>0.03052172590887187</v>
+      </c>
+      <c r="G68">
+        <v>0.001159436146043759</v>
+      </c>
+      <c r="H68">
+        <v>0.9634029792204588</v>
+      </c>
+      <c r="I68">
+        <v>0.03659702077954119</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>DE_27.05.2020</t>
+        </is>
+      </c>
+      <c r="C69" s="2">
+        <v>43978</v>
+      </c>
+      <c r="D69">
+        <v>0.04935663072613604</v>
+      </c>
+      <c r="E69">
+        <v>0.03156652432545901</v>
+      </c>
+      <c r="F69">
+        <v>0.03044311968379282</v>
+      </c>
+      <c r="G69">
+        <v>0.001123404641666186</v>
+      </c>
+      <c r="H69">
+        <v>0.9644115193017897</v>
+      </c>
+      <c r="I69">
+        <v>0.03558848069821038</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>DE_28.05.2020</t>
+        </is>
+      </c>
+      <c r="C70" s="2">
+        <v>43979</v>
+      </c>
+      <c r="D70">
+        <v>0.04925828245279967</v>
+      </c>
+      <c r="E70">
+        <v>0.03146817605212264</v>
+      </c>
+      <c r="F70">
+        <v>0.0304027673347576</v>
+      </c>
+      <c r="G70">
+        <v>0.001065408717365036</v>
+      </c>
+      <c r="H70">
+        <v>0.9661432961478182</v>
+      </c>
+      <c r="I70">
+        <v>0.0338567038521818</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>DE_29.05.2020</t>
+        </is>
+      </c>
+      <c r="C71" s="2">
+        <v>43980</v>
+      </c>
+      <c r="D71">
+        <v>0.04917554275391851</v>
+      </c>
+      <c r="E71">
+        <v>0.03138543635324148</v>
+      </c>
+      <c r="F71">
+        <v>0.03037610021215315</v>
+      </c>
+      <c r="G71">
+        <v>0.001009336141088331</v>
+      </c>
+      <c r="H71">
+        <v>0.9678406210533987</v>
+      </c>
+      <c r="I71">
+        <v>0.03215937894660135</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>DE_30.05.2020</t>
+        </is>
+      </c>
+      <c r="C72" s="2">
+        <v>43981</v>
+      </c>
+      <c r="D72">
+        <v>0.04909097604314203</v>
+      </c>
+      <c r="E72">
+        <v>0.03130086964246499</v>
+      </c>
+      <c r="F72">
+        <v>0.03032131343711715</v>
+      </c>
+      <c r="G72">
+        <v>0.0009795562053478437</v>
+      </c>
+      <c r="H72">
+        <v>0.9687051440890669</v>
+      </c>
+      <c r="I72">
+        <v>0.03129485591093315</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>DE_31.05.2020</t>
+        </is>
+      </c>
+      <c r="C73" s="2">
+        <v>43982</v>
+      </c>
+      <c r="D73">
+        <v>0.04905452766465396</v>
+      </c>
+      <c r="E73">
+        <v>0.03126442126397692</v>
+      </c>
+      <c r="F73">
+        <v>0.03029810054243242</v>
+      </c>
+      <c r="G73">
+        <v>0.0009663207215445128</v>
+      </c>
+      <c r="H73">
+        <v>0.9690920003480789</v>
+      </c>
+      <c r="I73">
+        <v>0.03090799965192108</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>DE_01.06.2020</t>
+        </is>
+      </c>
+      <c r="C74" s="2">
+        <v>43983</v>
+      </c>
+      <c r="D74">
+        <v>0.04904479216960014</v>
+      </c>
+      <c r="E74">
+        <v>0.03125468576892311</v>
+      </c>
+      <c r="F74">
+        <v>0.03029699820907453</v>
+      </c>
+      <c r="G74">
+        <v>0.0009576875598485782</v>
+      </c>
+      <c r="H74">
+        <v>0.9693585925985916</v>
+      </c>
+      <c r="I74">
+        <v>0.03064140740140852</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>DE_02.06.2020</t>
+        </is>
+      </c>
+      <c r="C75" s="2">
+        <v>43984</v>
+      </c>
+      <c r="D75">
+        <v>0.04899543178905163</v>
+      </c>
+      <c r="E75">
+        <v>0.0312053253883746</v>
+      </c>
+      <c r="F75">
+        <v>0.03026888286020747</v>
+      </c>
+      <c r="G75">
+        <v>0.0009364425281671315</v>
+      </c>
+      <c r="H75">
+        <v>0.9699909385173084</v>
+      </c>
+      <c r="I75">
+        <v>0.03000906148269163</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>DE_03.06.2020</t>
+        </is>
+      </c>
+      <c r="C76" s="2">
+        <v>43985</v>
+      </c>
+      <c r="D76">
+        <v>0.04891840231970322</v>
+      </c>
+      <c r="E76">
+        <v>0.03112829591902619</v>
+      </c>
+      <c r="F76">
+        <v>0.03019984735284887</v>
+      </c>
+      <c r="G76">
+        <v>0.0009284485661773203</v>
+      </c>
+      <c r="H76">
+        <v>0.9701734856096047</v>
+      </c>
+      <c r="I76">
+        <v>0.02982651439039538</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>DE_04.06.2020</t>
+        </is>
+      </c>
+      <c r="C77" s="2">
+        <v>43986</v>
+      </c>
+      <c r="D77">
+        <v>0.04881715627263963</v>
+      </c>
+      <c r="E77">
+        <v>0.0310270498719626</v>
+      </c>
+      <c r="F77">
+        <v>0.03011936843576621</v>
+      </c>
+      <c r="G77">
+        <v>0.0009076814361963843</v>
+      </c>
+      <c r="H77">
+        <v>0.9707454804777748</v>
+      </c>
+      <c r="I77">
+        <v>0.02925451952222519</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>DE_05.06.2020</t>
+        </is>
+      </c>
+      <c r="C78" s="2">
+        <v>43987</v>
+      </c>
+      <c r="D78">
+        <v>0.04873330362674028</v>
+      </c>
+      <c r="E78">
+        <v>0.03094319722606325</v>
+      </c>
+      <c r="F78">
+        <v>0.03006402815457187</v>
+      </c>
+      <c r="G78">
+        <v>0.0008791690714913793</v>
+      </c>
+      <c r="H78">
+        <v>0.9715876460642258</v>
+      </c>
+      <c r="I78">
+        <v>0.02841235393577432</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>DE_06.06.2020</t>
+        </is>
+      </c>
+      <c r="C79" s="2">
+        <v>43988</v>
+      </c>
+      <c r="D79">
+        <v>0.0486810100057568</v>
+      </c>
+      <c r="E79">
+        <v>0.03089090360507977</v>
+      </c>
+      <c r="F79">
+        <v>0.03002610302032497</v>
+      </c>
+      <c r="G79">
+        <v>0.0008648005847547987</v>
+      </c>
+      <c r="H79">
+        <v>0.9720046847508667</v>
+      </c>
+      <c r="I79">
+        <v>0.02799531524913337</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>DE_07.06.2020</t>
+        </is>
+      </c>
+      <c r="C80" s="2">
+        <v>43989</v>
+      </c>
+      <c r="D80">
+        <v>0.04865944083466058</v>
+      </c>
+      <c r="E80">
+        <v>0.03086933443398355</v>
+      </c>
+      <c r="F80">
+        <v>0.03001557223608773</v>
+      </c>
+      <c r="G80">
+        <v>0.0008537621978958246</v>
+      </c>
+      <c r="H80">
+        <v>0.9723427079478613</v>
+      </c>
+      <c r="I80">
+        <v>0.02765729205213869</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>DE_08.06.2020</t>
+        </is>
+      </c>
+      <c r="C81" s="2">
+        <v>43990</v>
+      </c>
+      <c r="D81">
+        <v>0.0485971141251989</v>
+      </c>
+      <c r="E81">
+        <v>0.03080700772452187</v>
+      </c>
+      <c r="F81">
+        <v>0.02996917474505946</v>
+      </c>
+      <c r="G81">
+        <v>0.0008378329794624076</v>
+      </c>
+      <c r="H81">
+        <v>0.9728038183080174</v>
+      </c>
+      <c r="I81">
+        <v>0.02719618169198258</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>DE_09.06.2020</t>
+        </is>
+      </c>
+      <c r="C82" s="2">
+        <v>43991</v>
+      </c>
+      <c r="D82">
+        <v>0.04849102726999297</v>
+      </c>
+      <c r="E82">
+        <v>0.03070092086931594</v>
+      </c>
+      <c r="F82">
+        <v>0.02990269492295086</v>
+      </c>
+      <c r="G82">
+        <v>0.0007982259463650774</v>
+      </c>
+      <c r="H82">
+        <v>0.9739999347328091</v>
+      </c>
+      <c r="I82">
+        <v>0.0260000652671909</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>DE_10.06.2020</t>
+        </is>
+      </c>
+      <c r="C83" s="2">
+        <v>43992</v>
+      </c>
+      <c r="D83">
+        <v>0.04839879573801971</v>
+      </c>
+      <c r="E83">
+        <v>0.03060868933734268</v>
+      </c>
+      <c r="F83">
+        <v>0.02982705733020355</v>
+      </c>
+      <c r="G83">
+        <v>0.0007816320071391301</v>
+      </c>
+      <c r="H83">
+        <v>0.9744637217711397</v>
+      </c>
+      <c r="I83">
+        <v>0.02553627822886023</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>DE_11.06.2020</t>
+        </is>
+      </c>
+      <c r="C84" s="2">
+        <v>43993</v>
+      </c>
+      <c r="D84">
+        <v>0.04833075337755551</v>
+      </c>
+      <c r="E84">
+        <v>0.03054064697687848</v>
+      </c>
+      <c r="F84">
+        <v>0.0297906110914054</v>
+      </c>
+      <c r="G84">
+        <v>0.0007500358854730864</v>
+      </c>
+      <c r="H84">
+        <v>0.9754413884538556</v>
+      </c>
+      <c r="I84">
+        <v>0.02455861154614435</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>DE_12.06.2020</t>
+        </is>
+      </c>
+      <c r="C85" s="2">
+        <v>43994</v>
+      </c>
+      <c r="D85">
+        <v>0.04829014876671747</v>
+      </c>
+      <c r="E85">
+        <v>0.03050004236604044</v>
+      </c>
+      <c r="F85">
+        <v>0.02977395414461483</v>
+      </c>
+      <c r="G85">
+        <v>0.0007260882214256126</v>
+      </c>
+      <c r="H85">
+        <v>0.9761938618736458</v>
+      </c>
+      <c r="I85">
+        <v>0.02380613812635416</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>DE_13.06.2020</t>
+        </is>
+      </c>
+      <c r="C86" s="2">
+        <v>43995</v>
+      </c>
+      <c r="D86">
+        <v>0.04821834837019947</v>
+      </c>
+      <c r="E86">
+        <v>0.03042824196952243</v>
+      </c>
+      <c r="F86">
+        <v>0.0297234373496305</v>
+      </c>
+      <c r="G86">
+        <v>0.0007048046198919233</v>
+      </c>
+      <c r="H86">
+        <v>0.9768371560671212</v>
+      </c>
+      <c r="I86">
+        <v>0.02316284393287889</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>DE_14.06.2020</t>
+        </is>
+      </c>
+      <c r="C87" s="2">
+        <v>43996</v>
+      </c>
+      <c r="D87">
+        <v>0.04820581891648389</v>
+      </c>
+      <c r="E87">
+        <v>0.03041571251580686</v>
+      </c>
+      <c r="F87">
+        <v>0.0297135988323088</v>
+      </c>
+      <c r="G87">
+        <v>0.0007021136834980707</v>
+      </c>
+      <c r="H87">
+        <v>0.9769160862783278</v>
+      </c>
+      <c r="I87">
+        <v>0.02308391372167219</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>DE_15.06.2020</t>
+        </is>
+      </c>
+      <c r="C88" s="2">
+        <v>43997</v>
+      </c>
+      <c r="D88">
+        <v>0.04816076039366837</v>
+      </c>
+      <c r="E88">
+        <v>0.03037065399299134</v>
+      </c>
+      <c r="F88">
+        <v>0.02968149711252126</v>
+      </c>
+      <c r="G88">
+        <v>0.0006891568804700851</v>
+      </c>
+      <c r="H88">
+        <v>0.9773084609692921</v>
+      </c>
+      <c r="I88">
+        <v>0.02269153903070781</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>DE_16.06.2020</t>
+        </is>
+      </c>
+      <c r="C89" s="2">
+        <v>43998</v>
+      </c>
+      <c r="D89">
+        <v>0.04806451956802166</v>
+      </c>
+      <c r="E89">
+        <v>0.03027441316734464</v>
+      </c>
+      <c r="F89">
+        <v>0.02959771851919006</v>
+      </c>
+      <c r="G89">
+        <v>0.000676694648154577</v>
+      </c>
+      <c r="H89">
+        <v>0.9776479681236401</v>
+      </c>
+      <c r="I89">
+        <v>0.0223520318763599</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>DE_17.06.2020</t>
+        </is>
+      </c>
+      <c r="C90" s="2">
+        <v>43999</v>
+      </c>
+      <c r="D90">
+        <v>0.04783846940653023</v>
+      </c>
+      <c r="E90">
+        <v>0.0300483630058532</v>
+      </c>
+      <c r="F90">
+        <v>0.02941317600620808</v>
+      </c>
+      <c r="G90">
+        <v>0.0006351869996451151</v>
+      </c>
+      <c r="H90">
+        <v>0.9788611779110434</v>
+      </c>
+      <c r="I90">
+        <v>0.02113882208895658</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>DE_18.06.2020</t>
+        </is>
+      </c>
+      <c r="C91" s="2">
+        <v>44000</v>
+      </c>
+      <c r="D91">
+        <v>0.04768422610239716</v>
+      </c>
+      <c r="E91">
+        <v>0.02989411970172013</v>
+      </c>
+      <c r="F91">
+        <v>0.02929329006926089</v>
+      </c>
+      <c r="G91">
+        <v>0.0006008296324592376</v>
+      </c>
+      <c r="H91">
+        <v>0.9799014107639147</v>
+      </c>
+      <c r="I91">
+        <v>0.0200985892360853</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>DE_19.06.2020</t>
+        </is>
+      </c>
+      <c r="C92" s="2">
+        <v>44001</v>
+      </c>
+      <c r="D92">
+        <v>0.0474915314860401</v>
+      </c>
+      <c r="E92">
+        <v>0.02970142508536307</v>
+      </c>
+      <c r="F92">
+        <v>0.02912047339372796</v>
+      </c>
+      <c r="G92">
+        <v>0.0005809516916351111</v>
+      </c>
+      <c r="H92">
+        <v>0.9804402755098305</v>
+      </c>
+      <c r="I92">
+        <v>0.01955972449016951</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>DE_20.06.2020</t>
+        </is>
+      </c>
+      <c r="C93" s="2">
+        <v>44002</v>
+      </c>
+      <c r="D93">
+        <v>0.04737526482342395</v>
+      </c>
+      <c r="E93">
+        <v>0.02958515842274692</v>
+      </c>
+      <c r="F93">
+        <v>0.02902294004327824</v>
+      </c>
+      <c r="G93">
+        <v>0.0005622183794686848</v>
+      </c>
+      <c r="H93">
+        <v>0.9809966074396135</v>
+      </c>
+      <c r="I93">
+        <v>0.0190033925603865</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>DE_21.06.2020</t>
+        </is>
+      </c>
+      <c r="C94" s="2">
+        <v>44003</v>
+      </c>
+      <c r="D94">
+        <v>0.04732141781440098</v>
+      </c>
+      <c r="E94">
+        <v>0.02953131141372395</v>
+      </c>
+      <c r="F94">
+        <v>0.02897715259926816</v>
+      </c>
+      <c r="G94">
+        <v>0.000554158814455783</v>
+      </c>
+      <c r="H94">
+        <v>0.9812348728205057</v>
+      </c>
+      <c r="I94">
+        <v>0.01876512717949435</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>DE_22.06.2020</t>
+        </is>
+      </c>
+      <c r="C95" s="2">
+        <v>44004</v>
+      </c>
+      <c r="D95">
+        <v>0.0472062573148303</v>
+      </c>
+      <c r="E95">
+        <v>0.02941615091415327</v>
+      </c>
+      <c r="F95">
+        <v>0.02888671903540374</v>
+      </c>
+      <c r="G95">
+        <v>0.0005294318787495253</v>
+      </c>
+      <c r="H95">
+        <v>0.9820020001836884</v>
+      </c>
+      <c r="I95">
+        <v>0.01799799981631162</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>DE_23.06.2020</t>
+        </is>
+      </c>
+      <c r="C96" s="2">
+        <v>44005</v>
+      </c>
+      <c r="D96">
+        <v>0.04708853346615662</v>
+      </c>
+      <c r="E96">
+        <v>0.02929842706547959</v>
+      </c>
+      <c r="F96">
+        <v>0.02879775199704968</v>
+      </c>
+      <c r="G96">
+        <v>0.0005006750684299159</v>
+      </c>
+      <c r="H96">
+        <v>0.9829111963140222</v>
+      </c>
+      <c r="I96">
+        <v>0.01708880368597768</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>DE_24.06.2020</t>
+        </is>
+      </c>
+      <c r="C97" s="2">
+        <v>44006</v>
+      </c>
+      <c r="D97">
+        <v>0.04697020166090807</v>
+      </c>
+      <c r="E97">
+        <v>0.02918009526023104</v>
+      </c>
+      <c r="F97">
+        <v>0.02870814683335379</v>
+      </c>
+      <c r="G97">
+        <v>0.0004719484268772527</v>
+      </c>
+      <c r="H97">
+        <v>0.9838263575677746</v>
+      </c>
+      <c r="I97">
+        <v>0.01617364243222542</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>DE_25.06.2020</t>
+        </is>
+      </c>
+      <c r="C98" s="2">
+        <v>44007</v>
+      </c>
+      <c r="D98">
+        <v>0.04684870466321243</v>
+      </c>
+      <c r="E98">
+        <v>0.02905859826253541</v>
+      </c>
+      <c r="F98">
+        <v>0.02862356643062038</v>
+      </c>
+      <c r="G98">
+        <v>0.0004350318319150274</v>
+      </c>
+      <c r="H98">
+        <v>0.9850291528867067</v>
+      </c>
+      <c r="I98">
+        <v>0.01497084711329328</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>DE_26.06.2020</t>
+        </is>
+      </c>
+      <c r="C99" s="2">
+        <v>44008</v>
+      </c>
+      <c r="D99">
+        <v>0.04673107213353742</v>
+      </c>
+      <c r="E99">
+        <v>0.02894096573286039</v>
+      </c>
+      <c r="F99">
+        <v>0.02852641286219352</v>
+      </c>
+      <c r="G99">
+        <v>0.000414552870666872</v>
+      </c>
+      <c r="H99">
+        <v>0.9856759143943779</v>
+      </c>
+      <c r="I99">
+        <v>0.01432408560562224</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>DE_27.06.2020</t>
+        </is>
+      </c>
+      <c r="C100" s="2">
+        <v>44009</v>
+      </c>
+      <c r="D100">
+        <v>0.04666031671050955</v>
+      </c>
+      <c r="E100">
+        <v>0.02887021030983252</v>
+      </c>
+      <c r="F100">
+        <v>0.02845903850031286</v>
+      </c>
+      <c r="G100">
+        <v>0.000411171809519662</v>
+      </c>
+      <c r="H100">
+        <v>0.9857579212237458</v>
+      </c>
+      <c r="I100">
+        <v>0.01424207877625424</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>DE_28.06.2020</t>
+        </is>
+      </c>
+      <c r="C101" s="2">
+        <v>44010</v>
+      </c>
+      <c r="D101">
+        <v>0.04661272133701441</v>
+      </c>
+      <c r="E101">
+        <v>0.02882261493633738</v>
+      </c>
+      <c r="F101">
+        <v>0.02842397784802368</v>
+      </c>
+      <c r="G101">
+        <v>0.0003986370883136934</v>
+      </c>
+      <c r="H101">
+        <v>0.9861692948681377</v>
+      </c>
+      <c r="I101">
+        <v>0.01383070513186234</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>DE_29.06.2020</t>
+        </is>
+      </c>
+      <c r="C102" s="2">
+        <v>44011</v>
+      </c>
+      <c r="D102">
+        <v>0.04652261461011305</v>
+      </c>
+      <c r="E102">
+        <v>0.02873250820943602</v>
+      </c>
+      <c r="F102">
+        <v>0.0283534746268929</v>
+      </c>
+      <c r="G102">
+        <v>0.0003790335825431217</v>
+      </c>
+      <c r="H102">
+        <v>0.9868081971897377</v>
+      </c>
+      <c r="I102">
+        <v>0.01319180281026227</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>DE_30.06.2020</t>
+        </is>
+      </c>
+      <c r="C103" s="2">
+        <v>44012</v>
+      </c>
+      <c r="D103">
+        <v>0.04641945524453683</v>
+      </c>
+      <c r="E103">
+        <v>0.0286293488438598</v>
+      </c>
+      <c r="F103">
+        <v>0.0282801559993603</v>
+      </c>
+      <c r="G103">
+        <v>0.0003491928444994996</v>
+      </c>
+      <c r="H103">
+        <v>0.9878029763651299</v>
+      </c>
+      <c r="I103">
+        <v>0.01219702363487012</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>DE_01.07.2020</t>
+        </is>
+      </c>
+      <c r="C104" s="2">
+        <v>44013</v>
+      </c>
+      <c r="D104">
+        <v>0.04631518308589507</v>
+      </c>
+      <c r="E104">
+        <v>0.02852507668521804</v>
+      </c>
+      <c r="F104">
+        <v>0.02820672011022286</v>
+      </c>
+      <c r="G104">
+        <v>0.0003183565749951818</v>
+      </c>
+      <c r="H104">
+        <v>0.9888394138775389</v>
+      </c>
+      <c r="I104">
+        <v>0.01116058612246105</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>DE_02.07.2020</t>
+        </is>
+      </c>
+      <c r="C105" s="2">
+        <v>44014</v>
+      </c>
+      <c r="D105">
+        <v>0.0462208484812603</v>
+      </c>
+      <c r="E105">
+        <v>0.02843074208058327</v>
+      </c>
+      <c r="F105">
+        <v>0.02812573317714611</v>
+      </c>
+      <c r="G105">
+        <v>0.0003050089034371552</v>
+      </c>
+      <c r="H105">
+        <v>0.9892718627402463</v>
+      </c>
+      <c r="I105">
+        <v>0.01072813725975379</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>DE_03.07.2020</t>
+        </is>
+      </c>
+      <c r="C106" s="2">
+        <v>44015</v>
+      </c>
+      <c r="D106">
+        <v>0.04613597403033937</v>
+      </c>
+      <c r="E106">
+        <v>0.02834586762966234</v>
+      </c>
+      <c r="F106">
+        <v>0.02805133024022129</v>
+      </c>
+      <c r="G106">
+        <v>0.0002945373894410507</v>
+      </c>
+      <c r="H106">
+        <v>0.9896091594976323</v>
+      </c>
+      <c r="I106">
+        <v>0.01039084050236776</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>DE_04.07.2020</t>
+        </is>
+      </c>
+      <c r="C107" s="2">
+        <v>44016</v>
+      </c>
+      <c r="D107">
+        <v>0.04606681007083759</v>
+      </c>
+      <c r="E107">
+        <v>0.02827670367016056</v>
+      </c>
+      <c r="F107">
+        <v>0.02800716129654455</v>
+      </c>
+      <c r="G107">
+        <v>0.000269542373616009</v>
+      </c>
+      <c r="H107">
+        <v>0.9904676875791415</v>
+      </c>
+      <c r="I107">
+        <v>0.009532312420858584</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>DE_05.07.2020</t>
+        </is>
+      </c>
+      <c r="C108" s="2">
+        <v>44017</v>
+      </c>
+      <c r="D108">
+        <v>0.04603356894948396</v>
+      </c>
+      <c r="E108">
+        <v>0.02824346254880693</v>
+      </c>
+      <c r="F108">
+        <v>0.02798080887382245</v>
+      </c>
+      <c r="G108">
+        <v>0.0002626536749844799</v>
+      </c>
+      <c r="H108">
+        <v>0.9907003727134874</v>
+      </c>
+      <c r="I108">
+        <v>0.009299627286512539</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>DE_06.07.2020</t>
+        </is>
+      </c>
+      <c r="C109" s="2">
+        <v>44018</v>
+      </c>
+      <c r="D109">
+        <v>0.04596600710299341</v>
+      </c>
+      <c r="E109">
+        <v>0.02817590070231638</v>
+      </c>
+      <c r="F109">
+        <v>0.02792635111758996</v>
+      </c>
+      <c r="G109">
+        <v>0.0002495495847264073</v>
+      </c>
+      <c r="H109">
+        <v>0.9911431550187891</v>
+      </c>
+      <c r="I109">
+        <v>0.008856844981210896</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>DE_07.07.2020</t>
+        </is>
+      </c>
+      <c r="C110" s="2">
+        <v>44019</v>
+      </c>
+      <c r="D110">
+        <v>0.04588029773659426</v>
+      </c>
+      <c r="E110">
+        <v>0.02809019133591723</v>
+      </c>
+      <c r="F110">
+        <v>0.02786035973014728</v>
+      </c>
+      <c r="G110">
+        <v>0.0002298316057699452</v>
+      </c>
+      <c r="H110">
+        <v>0.9918180832938623</v>
+      </c>
+      <c r="I110">
+        <v>0.008181916706137684</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>DE_08.07.2020</t>
+        </is>
+      </c>
+      <c r="C111" s="2">
+        <v>44020</v>
+      </c>
+      <c r="D111">
+        <v>0.04579253690624147</v>
+      </c>
+      <c r="E111">
+        <v>0.02800243050556444</v>
+      </c>
+      <c r="F111">
+        <v>0.02779204554082868</v>
+      </c>
+      <c r="G111">
+        <v>0.00021038496473576</v>
+      </c>
+      <c r="H111">
+        <v>0.9924869034245454</v>
+      </c>
+      <c r="I111">
+        <v>0.007513096575454541</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>DE_09.07.2020</t>
+        </is>
+      </c>
+      <c r="C112" s="2">
+        <v>44021</v>
+      </c>
+      <c r="D112">
+        <v>0.0456979014731484</v>
+      </c>
+      <c r="E112">
+        <v>0.02790779507247137</v>
+      </c>
+      <c r="F112">
+        <v>0.027719918467431</v>
+      </c>
+      <c r="G112">
+        <v>0.0001878766050403799</v>
+      </c>
+      <c r="H112">
+        <v>0.9932679523927813</v>
+      </c>
+      <c r="I112">
+        <v>0.00673204760721867</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>DE_10.07.2020</t>
+        </is>
+      </c>
+      <c r="C113" s="2">
+        <v>44022</v>
+      </c>
+      <c r="D113">
+        <v>0.04561650909068948</v>
+      </c>
+      <c r="E113">
+        <v>0.02782640269001245</v>
+      </c>
+      <c r="F113">
+        <v>0.02765551729485361</v>
+      </c>
+      <c r="G113">
+        <v>0.0001708853951588322</v>
+      </c>
+      <c r="H113">
+        <v>0.9938588757928035</v>
+      </c>
+      <c r="I113">
+        <v>0.006141124207196463</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>DE_11.07.2020</t>
+        </is>
+      </c>
+      <c r="C114" s="2">
+        <v>44023</v>
+      </c>
+      <c r="D114">
+        <v>0.04556832584326716</v>
+      </c>
+      <c r="E114">
+        <v>0.02777821944259013</v>
+      </c>
+      <c r="F114">
+        <v>0.02761672596520955</v>
+      </c>
+      <c r="G114">
+        <v>0.0001614934773805753</v>
+      </c>
+      <c r="H114">
+        <v>0.994186327251308</v>
+      </c>
+      <c r="I114">
+        <v>0.005813672748692099</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>DE_12.07.2020</t>
+        </is>
+      </c>
+      <c r="C115" s="2">
+        <v>44024</v>
+      </c>
+      <c r="D115">
+        <v>0.0455557063373592</v>
+      </c>
+      <c r="E115">
+        <v>0.02776559993668218</v>
+      </c>
+      <c r="F115">
+        <v>0.0276094240280651</v>
+      </c>
+      <c r="G115">
+        <v>0.000156175908617081</v>
+      </c>
+      <c r="H115">
+        <v>0.9943752013652422</v>
+      </c>
+      <c r="I115">
+        <v>0.005624798634757795</v>
       </c>
     </row>
   </sheetData>

</xml_diff>